<commit_message>
extracting all details for a particular match in the given url
</commit_message>
<xml_diff>
--- a/tmp/batsmendata.xlsx
+++ b/tmp/batsmendata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>BATSMEN</t>
   </si>
@@ -236,6 +236,48 @@
   </si>
   <si>
     <t>(nb 8)</t>
+  </si>
+  <si>
+    <t>KS Bharat †</t>
+  </si>
+  <si>
+    <t>lbw b Dhawan</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>42.85</t>
+  </si>
+  <si>
+    <t>DB Prasanth</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>48.69</t>
+  </si>
+  <si>
+    <t>GH Vihari (c)</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>45.63</t>
   </si>
 </sst>
 </file>
@@ -604,80 +646,80 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9">

</xml_diff>